<commit_message>
Update bot with auto-resize columns, history features, and HTML formatting fixes
</commit_message>
<xml_diff>
--- a/Расходники 9 октября.xlsx
+++ b/Расходники 9 октября.xlsx
@@ -432,6 +432,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
+    <col width="24" customWidth="1" min="4" max="4"/>
+    <col width="44" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -497,7 +506,9 @@
       <c r="F2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -526,7 +537,9 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -555,7 +568,9 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -582,9 +597,11 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -613,7 +630,9 @@
       <c r="F6" t="n">
         <v>1</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -624,7 +643,6 @@
           <t>Термоконтроллер Китай, 1300 С</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -638,7 +656,9 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -649,7 +669,6 @@
           <t>Термоконтроллер Китай, 400 С</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -663,7 +682,9 @@
       <c r="F8" t="n">
         <v>10</v>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -690,9 +711,11 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>12</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -721,7 +744,9 @@
       <c r="F10" t="n">
         <v>1</v>
       </c>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -748,9 +773,11 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -779,7 +806,9 @@
       <c r="F12" t="n">
         <v>6</v>
       </c>
-      <c r="G12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -808,7 +837,9 @@
       <c r="F13" t="n">
         <v>1</v>
       </c>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -837,7 +868,9 @@
       <c r="F14" t="n">
         <v>3</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -866,7 +899,9 @@
       <c r="F15" t="n">
         <v>3</v>
       </c>
-      <c r="G15" t="inlineStr"/>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -895,7 +930,9 @@
       <c r="F16" t="n">
         <v>4</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -924,7 +961,9 @@
       <c r="F17" t="n">
         <v>2</v>
       </c>
-      <c r="G17" t="inlineStr"/>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -953,7 +992,9 @@
       <c r="F18" t="n">
         <v>4</v>
       </c>
-      <c r="G18" t="inlineStr"/>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -982,7 +1023,9 @@
       <c r="F19" t="n">
         <v>6</v>
       </c>
-      <c r="G19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -993,7 +1036,6 @@
           <t>Таймер DH48S-S AC 220 В 5 А</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1007,7 +1049,9 @@
       <c r="F20" t="n">
         <v>0</v>
       </c>
-      <c r="G20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1034,9 +1078,11 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>8</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1065,7 +1111,9 @@
       <c r="F22" t="n">
         <v>9</v>
       </c>
-      <c r="G22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1094,7 +1142,9 @@
       <c r="F23" t="n">
         <v>13</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1123,7 +1173,9 @@
       <c r="F24" t="n">
         <v>4</v>
       </c>
-      <c r="G24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1152,7 +1204,9 @@
       <c r="F25" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1181,7 +1235,9 @@
       <c r="F26" t="n">
         <v>29</v>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1210,7 +1266,9 @@
       <c r="F27" t="n">
         <v>12</v>
       </c>
-      <c r="G27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1221,7 +1279,6 @@
           <t>Сигнальные лампы</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1235,7 +1292,9 @@
       <c r="F28" t="n">
         <v>20</v>
       </c>
-      <c r="G28" t="inlineStr"/>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1246,7 +1305,6 @@
           <t>Вилки для розеток черный</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1260,7 +1318,9 @@
       <c r="F29" t="n">
         <v>8</v>
       </c>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1289,7 +1349,9 @@
       <c r="F30" t="n">
         <v>3</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1318,7 +1380,9 @@
       <c r="F31" t="n">
         <v>9</v>
       </c>
-      <c r="G31" t="inlineStr"/>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1347,7 +1411,9 @@
       <c r="F32" t="n">
         <v>9</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1376,7 +1442,9 @@
       <c r="F33" t="n">
         <v>2</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1405,7 +1473,9 @@
       <c r="F34" t="n">
         <v>3</v>
       </c>
-      <c r="G34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1434,7 +1504,9 @@
       <c r="F35" t="n">
         <v>11</v>
       </c>
-      <c r="G35" t="inlineStr"/>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1463,7 +1535,9 @@
       <c r="F36" t="n">
         <v>11</v>
       </c>
-      <c r="G36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1492,7 +1566,9 @@
       <c r="F37" t="n">
         <v>12</v>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1521,7 +1597,9 @@
       <c r="F38" t="n">
         <v>28</v>
       </c>
-      <c r="G38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1550,7 +1628,9 @@
       <c r="F39" t="n">
         <v>18</v>
       </c>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1579,7 +1659,9 @@
       <c r="F40" t="n">
         <v>7</v>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1608,7 +1690,9 @@
       <c r="F41" t="n">
         <v>8</v>
       </c>
-      <c r="G41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1637,7 +1721,9 @@
       <c r="F42" t="n">
         <v>3</v>
       </c>
-      <c r="G42" t="inlineStr"/>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1666,7 +1752,9 @@
       <c r="F43" t="n">
         <v>2</v>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1677,7 +1765,6 @@
           <t>Кнопки включения, 220 В</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1691,7 +1778,9 @@
       <c r="F44" t="n">
         <v>9</v>
       </c>
-      <c r="G44" t="inlineStr"/>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1702,7 +1791,6 @@
           <t>Кнопки включения, 12-24 В</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1716,7 +1804,9 @@
       <c r="F45" t="n">
         <v>3</v>
       </c>
-      <c r="G45" t="inlineStr"/>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1727,7 +1817,6 @@
           <t xml:space="preserve">Концевик </t>
         </is>
       </c>
-      <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr">
         <is>
           <t>Китай</t>
@@ -1741,7 +1830,9 @@
       <c r="F46" t="n">
         <v>6</v>
       </c>
-      <c r="G46" t="inlineStr"/>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1770,7 +1861,9 @@
       <c r="F47" t="n">
         <v>9</v>
       </c>
-      <c r="G47" t="inlineStr"/>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1799,7 +1892,9 @@
       <c r="F48" t="n">
         <v>10</v>
       </c>
-      <c r="G48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1828,7 +1923,9 @@
       <c r="F49" t="n">
         <v>8</v>
       </c>
-      <c r="G49" t="inlineStr"/>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1857,7 +1954,9 @@
       <c r="F50" t="n">
         <v>7</v>
       </c>
-      <c r="G50" t="inlineStr"/>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1886,7 +1985,9 @@
       <c r="F51" t="n">
         <v>13</v>
       </c>
-      <c r="G51" t="inlineStr"/>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1913,7 +2014,9 @@
       <c r="F52" t="n">
         <v>3</v>
       </c>
-      <c r="G52" t="inlineStr"/>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1940,7 +2043,9 @@
       <c r="F53" t="n">
         <v>3</v>
       </c>
-      <c r="G53" t="inlineStr"/>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1967,7 +2072,9 @@
       <c r="F54" t="n">
         <v>4</v>
       </c>
-      <c r="G54" t="inlineStr"/>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1994,7 +2101,9 @@
       <c r="F55" t="n">
         <v>3</v>
       </c>
-      <c r="G55" t="inlineStr"/>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -2021,7 +2130,9 @@
       <c r="F56" t="n">
         <v>3</v>
       </c>
-      <c r="G56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -2048,7 +2159,9 @@
       <c r="F57" t="n">
         <v>3</v>
       </c>
-      <c r="G57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -2075,7 +2188,9 @@
       <c r="F58" t="n">
         <v>2</v>
       </c>
-      <c r="G58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -2102,7 +2217,9 @@
       <c r="F59" t="n">
         <v>1</v>
       </c>
-      <c r="G59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -2113,17 +2230,17 @@
           <t>Зажимы крокодил</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
       <c r="D60" t="inlineStr">
         <is>
           <t>Китай</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
         <v>12</v>
       </c>
-      <c r="G60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -2152,7 +2269,9 @@
       <c r="F61" t="n">
         <v>2</v>
       </c>
-      <c r="G61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2181,7 +2300,9 @@
       <c r="F62" t="n">
         <v>3</v>
       </c>
-      <c r="G62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>